<commit_message>
WEEK 05-11 Last edit
</commit_message>
<xml_diff>
--- a/WEEK formos/WEEK 05-11.xlsx
+++ b/WEEK formos/WEEK 05-11.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDYING\Semester_6\Team_Software_Process\Cycle_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaponnik\Desktop\git repos\TSP\WEEK formos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{652CD3F8-C022-4C85-B639-09666944E556}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BECE1CB5-2C96-47B5-AF3F-C1A1D7FD30FD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27374" windowHeight="11164" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27375" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week" sheetId="1" r:id="rId1"/>
@@ -358,13 +358,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>153909</xdr:rowOff>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>72428</xdr:colOff>
+          <xdr:colOff>76200</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>18107</xdr:rowOff>
+          <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -921,27 +921,27 @@
   <sheetPr codeName="WeekSummary"/>
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.75" style="3" customWidth="1"/>
-    <col min="2" max="2" width="0.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="0.875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.75" style="4" customWidth="1"/>
-    <col min="6" max="6" width="0.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.75" style="4" customWidth="1"/>
-    <col min="8" max="8" width="0.875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.75" style="3" customWidth="1"/>
-    <col min="10" max="10" width="1.75" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.125" style="2"/>
-    <col min="12" max="16384" width="9.125" style="1"/>
+    <col min="1" max="1" width="30.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="0.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="0.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="0.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="0.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="3" customWidth="1"/>
+    <col min="10" max="10" width="1.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="str">
         <f>[0]!TSPProcessName &amp; " Week Summary - Form WEEK"</f>
         <v>TSPi Week Summary - Form WEEK</v>
@@ -951,7 +951,7 @@
       <c r="G1" s="9"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:11" s="16" customFormat="1" ht="12.85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>26</v>
       </c>
@@ -972,7 +972,7 @@
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
     </row>
-    <row r="3" spans="1:11" s="16" customFormat="1" ht="12.85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>23</v>
       </c>
@@ -994,7 +994,7 @@
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
     </row>
-    <row r="4" spans="1:11" s="16" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" s="16" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>20</v>
       </c>
@@ -1114,7 +1114,7 @@
       <c r="G13" s="9"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="24.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>9</v>
       </c>
       <c r="I15" s="5">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1204,7 +1204,7 @@
         <v>8</v>
       </c>
       <c r="I18" s="5">
-        <v>6.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1223,7 +1223,7 @@
         <v>8</v>
       </c>
       <c r="I19" s="5">
-        <v>6.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1473,13 +1473,13 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>153909</xdr:rowOff>
+                    <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>72428</xdr:colOff>
+                    <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>18107</xdr:rowOff>
+                    <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>